<commit_message>
Take screenshot and Iretry run
</commit_message>
<xml_diff>
--- a/src/main/resources/Data_Engine/Driver_File.xlsx
+++ b/src/main/resources/Data_Engine/Driver_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanmugasundharam\Git\Selenium_Hybrid_Framework\Selenium\src\main\resources\Data_Engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shanmugasundharam\Git\S2_Application\Selenium\src\main\resources\Data_Engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF66121-67BE-4725-8230-6CFEC8F3917C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2231E2FF-0B58-457F-9078-7ABA68DD0287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>S No</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Action Keyword</t>
-  </si>
-  <si>
-    <t>TestSuite1()</t>
   </si>
   <si>
     <t>TestSuite2()</t>
@@ -381,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,11 +440,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>